<commit_message>
Ja Cansei de CODAR
</commit_message>
<xml_diff>
--- a/Modelagem_Fisica.xlsx
+++ b/Modelagem_Fisica.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\47218236812\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\47218236812\Desktop\s2019-sprint-1-bd_OPFlix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EAF8A60-88F8-4681-8360-EDD856EE41C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CC11F9-6529-4BDE-8FBA-2B01763C51A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{74598614-4E3B-40DD-B099-D0144D6B5981}"/>
   </bookViews>
@@ -42,39 +42,6 @@
     <t>Senha</t>
   </si>
   <si>
-    <t>Tipo</t>
-  </si>
-  <si>
-    <t>Lucas</t>
-  </si>
-  <si>
-    <t>Gustavo</t>
-  </si>
-  <si>
-    <t>Guilherme</t>
-  </si>
-  <si>
-    <t>Gabriel</t>
-  </si>
-  <si>
-    <t>Mariana</t>
-  </si>
-  <si>
-    <t>lucas@gmail.com</t>
-  </si>
-  <si>
-    <t>gustavo@gmail.com</t>
-  </si>
-  <si>
-    <t>guilherme@gmail.com</t>
-  </si>
-  <si>
-    <t>gabriel@gmail.com</t>
-  </si>
-  <si>
-    <t>mariana@gmail.com</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -136,6 +103,39 @@
   </si>
   <si>
     <t>Grey`s Anatomy</t>
+  </si>
+  <si>
+    <t>Erik</t>
+  </si>
+  <si>
+    <t>Cassiana</t>
+  </si>
+  <si>
+    <t>Helena</t>
+  </si>
+  <si>
+    <t>Roberto</t>
+  </si>
+  <si>
+    <t>erik@gmail.com</t>
+  </si>
+  <si>
+    <t>cassiana@gmail.com</t>
+  </si>
+  <si>
+    <t>helena@gmail.com</t>
+  </si>
+  <si>
+    <t>TipoFilme/Serie</t>
+  </si>
+  <si>
+    <t>TipoCategoria</t>
+  </si>
+  <si>
+    <t>Permissao</t>
+  </si>
+  <si>
+    <t>rob@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -159,7 +159,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,8 +226,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -250,16 +262,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -269,31 +324,23 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -611,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77EEE7A2-F5DE-4E58-BB8E-E7F2C90A2050}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,141 +669,143 @@
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="3"/>
+      <c r="G1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="10"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="6"/>
+      <c r="K1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="12"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>18</v>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="8">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3">
         <v>123456</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="3">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="9">
-        <v>1</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>19</v>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="5">
-        <v>1</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>24</v>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="8">
-        <v>654321</v>
-      </c>
-      <c r="E4" s="8">
-        <v>2</v>
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3">
+        <v>123456</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="9">
-        <v>2</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>20</v>
+      <c r="G4" s="4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="5">
-        <v>2</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>35</v>
+      <c r="K4" s="2">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="8">
-        <v>1357911</v>
-      </c>
-      <c r="E5" s="8">
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3">
+        <v>123456</v>
+      </c>
+      <c r="E5" s="3">
         <v>2</v>
       </c>
       <c r="F5" s="1"/>
@@ -764,27 +813,27 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="5">
+      <c r="K5" s="2">
         <v>3</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>25</v>
+      <c r="L5" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="8">
-        <v>246810</v>
-      </c>
-      <c r="E6" s="8">
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3110</v>
+      </c>
+      <c r="E6" s="3">
         <v>2</v>
       </c>
       <c r="F6" s="1"/>
@@ -792,47 +841,27 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="5">
+      <c r="K6" s="2">
         <v>4</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>31</v>
+      <c r="L6" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="8">
-        <v>112233</v>
-      </c>
-      <c r="E7" s="8">
-        <v>2</v>
-      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="5">
+      <c r="K7" s="2">
         <v>5</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>33</v>
+      <c r="L7" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -842,10 +871,10 @@
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="4"/>
+      <c r="A9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="11"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -858,10 +887,10 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="1"/>
@@ -876,11 +905,11 @@
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
-        <v>1</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>16</v>
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -894,11 +923,11 @@
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
-        <v>2</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>17</v>
+      <c r="A12" s="6">
+        <v>2</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -926,167 +955,189 @@
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="A14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="J14" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="16"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="12" t="s">
+      <c r="A15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="B15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="15"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="J15" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>1</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="13">
+      <c r="A16" s="7">
+        <v>1</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="8">
         <f>DATE(2019,6,26)</f>
         <v>43642</v>
       </c>
-      <c r="D16" s="12">
-        <v>1</v>
-      </c>
-      <c r="E16" s="12">
-        <v>3</v>
-      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="J16" s="18">
+        <v>1</v>
+      </c>
+      <c r="K16" s="18">
+        <v>3</v>
+      </c>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
-        <v>2</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="13">
+      <c r="A17" s="7">
+        <v>2</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="8">
         <f>DATE(2005,9,22)</f>
         <v>38617</v>
       </c>
-      <c r="D17" s="12">
-        <v>2</v>
-      </c>
-      <c r="E17" s="12">
-        <v>1</v>
-      </c>
+      <c r="D17" s="7">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="J17" s="18">
+        <v>2</v>
+      </c>
+      <c r="K17" s="18">
+        <v>1</v>
+      </c>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="A18" s="7">
         <v>3</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="13">
+      <c r="B18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="8">
         <v>43216</v>
       </c>
-      <c r="D18" s="12">
-        <v>1</v>
-      </c>
-      <c r="E18" s="12">
-        <v>4</v>
-      </c>
+      <c r="D18" s="7">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="J18" s="18">
+        <v>3</v>
+      </c>
+      <c r="K18" s="18">
+        <v>4</v>
+      </c>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+      <c r="A19" s="7">
         <v>4</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="13">
+      <c r="B19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="8">
         <v>35811</v>
       </c>
-      <c r="D19" s="12">
-        <v>1</v>
-      </c>
-      <c r="E19" s="12">
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
+      <c r="J19" s="18">
+        <v>4</v>
+      </c>
+      <c r="K19" s="18">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="A20" s="7">
         <v>5</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="13">
+      <c r="B20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="8">
         <v>38438</v>
       </c>
-      <c r="D20" s="12">
-        <v>2</v>
-      </c>
-      <c r="E20" s="12">
-        <v>2</v>
-      </c>
+      <c r="D20" s="7">
+        <v>2</v>
+      </c>
+      <c r="J20" s="18">
+        <v>5</v>
+      </c>
+      <c r="K20" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="A14:E14"/>
+    <mergeCell ref="J14:K14"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{BDACB7E6-E12C-4C11-B4A0-5FA413250228}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{BC3F90DE-F07C-46D1-A18F-0B6EC42C8C7F}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{9CCDBC7D-4A75-45E0-9E1B-E55AA2B6F556}"/>
-    <hyperlink ref="C6" r:id="rId4" xr:uid="{2A371DB2-B991-451A-A491-C655517A13A4}"/>
-    <hyperlink ref="C7" r:id="rId5" xr:uid="{0EFB53F1-D5D6-40A8-99F3-6A51F82BD634}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{A6E882FC-4979-49C1-94BC-99839842BA29}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{40ACFA9B-7848-45AB-981E-55E6B5BA8AA5}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{26FF8BF3-9A9C-44DB-A3B6-915D2230AE02}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{EFB5999F-1767-439B-8FBE-9D655C602661}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>